<commit_message>
Updating Existing data program
</commit_message>
<xml_diff>
--- a/File/TestData.xlsx
+++ b/File/TestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srmohan\eclipse-workspace\JavaAssignment\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6710D77C-893E-443D-8947-16FAB53170AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8D04DC-A35B-48FE-AE6B-FA99FE9519DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,27 +25,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Sl.No</t>
-  </si>
-  <si>
-    <t>Account Num</t>
-  </si>
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>Address</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>TC_DESC</t>
+  </si>
+  <si>
+    <t>TC_Status</t>
+  </si>
+  <si>
+    <t>qww</t>
+  </si>
+  <si>
+    <t>eee</t>
+  </si>
+  <si>
+    <t>fff</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,18 +370,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.7265625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,11 +388,38 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>